<commit_message>
MIDI Out Testing 2
Fixed IRQ issue - Simultaneous RX and TX now work.
</commit_message>
<xml_diff>
--- a/Docs/Keyboard Codes.xlsx
+++ b/Docs/Keyboard Codes.xlsx
@@ -30,9 +30,6 @@
     <t>No key Pressed</t>
   </si>
   <si>
-    <t>Middle C (C5)</t>
-  </si>
-  <si>
     <t>;</t>
   </si>
   <si>
@@ -41,12 +38,15 @@
   <si>
     <t>Select this part!</t>
   </si>
+  <si>
+    <t>Q=Middle C (C5)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,8 +54,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -65,6 +71,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -87,14 +99,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -400,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:J260"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,7 +435,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="4:10" x14ac:dyDescent="0.25">
@@ -428,7 +444,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>2</v>
@@ -444,13 +460,13 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -460,14 +476,14 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G6" s="1">
         <f>G14+1</f>
         <v>63</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I6" s="1"/>
     </row>
@@ -477,14 +493,14 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1">
         <f>G15+1</f>
         <v>66</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -494,14 +510,14 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G8" s="1">
         <f>G16+1</f>
         <v>70</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -511,14 +527,14 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G9" s="1">
         <f>G17+1</f>
         <v>73</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I9" s="1"/>
     </row>
@@ -528,13 +544,13 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I10" s="1"/>
     </row>
@@ -544,14 +560,14 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G11" s="1">
         <f>G19+1</f>
         <v>80</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -561,14 +577,14 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G12" s="1">
         <f>G67+1</f>
         <v>83</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I12" s="1"/>
     </row>
@@ -578,13 +594,13 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I13" s="1"/>
     </row>
@@ -594,14 +610,14 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G14" s="1">
         <f>G61+1</f>
         <v>62</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I14" s="1"/>
     </row>
@@ -611,14 +627,14 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G15" s="1">
         <f>G54+1</f>
         <v>65</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I15" s="1"/>
     </row>
@@ -628,14 +644,14 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G16" s="1">
         <f>G63+1</f>
         <v>69</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -645,14 +661,14 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G17" s="1">
         <f>G56+1</f>
         <v>72</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I17" s="1"/>
     </row>
@@ -662,14 +678,14 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G18" s="1">
         <f>G65+1</f>
         <v>76</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -679,14 +695,14 @@
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G19" s="1">
         <f>G66+1</f>
         <v>79</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I19" s="1"/>
     </row>
@@ -696,13 +712,13 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I20" s="1"/>
     </row>
@@ -712,13 +728,13 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G21" s="1">
         <v>0</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I21" s="1"/>
     </row>
@@ -728,13 +744,13 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G22" s="1">
         <v>0</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I22" s="1"/>
     </row>
@@ -744,13 +760,13 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G23" s="1">
         <v>0</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I23" s="1"/>
     </row>
@@ -760,13 +776,13 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G24" s="1">
         <v>0</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I24" s="1"/>
     </row>
@@ -776,13 +792,13 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G25" s="1">
         <v>0</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I25" s="1"/>
     </row>
@@ -792,13 +808,13 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G26" s="1">
         <v>0</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I26" s="1"/>
     </row>
@@ -808,13 +824,13 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G27" s="1">
         <v>0</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I27" s="1"/>
     </row>
@@ -824,13 +840,13 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G28" s="1">
         <v>0</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I28" s="1"/>
     </row>
@@ -840,13 +856,13 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G29" s="1">
         <v>0</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I29" s="1"/>
     </row>
@@ -856,13 +872,13 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G30" s="1">
         <v>0</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I30" s="1"/>
     </row>
@@ -872,13 +888,13 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G31" s="1">
         <v>0</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I31" s="1"/>
     </row>
@@ -888,13 +904,13 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G32" s="1">
         <v>0</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I32" s="1"/>
     </row>
@@ -904,13 +920,13 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G33" s="1">
         <v>0</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I33" s="1"/>
     </row>
@@ -920,13 +936,13 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G34" s="1">
         <v>0</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I34" s="1"/>
     </row>
@@ -936,13 +952,13 @@
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G35" s="1">
         <v>0</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I35" s="1"/>
     </row>
@@ -952,13 +968,13 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G36" s="1">
         <v>0</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I36" s="1"/>
     </row>
@@ -968,13 +984,13 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G37" s="1">
         <v>0</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I37" s="1"/>
     </row>
@@ -984,13 +1000,13 @@
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G38" s="1">
         <v>0</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I38" s="1"/>
     </row>
@@ -1000,13 +1016,13 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G39" s="1">
         <v>0</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I39" s="1"/>
     </row>
@@ -1016,13 +1032,13 @@
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G40" s="1">
         <v>0</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I40" s="1"/>
     </row>
@@ -1032,13 +1048,13 @@
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G41" s="1">
         <v>0</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I41" s="1"/>
     </row>
@@ -1048,13 +1064,13 @@
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G42" s="1">
         <v>0</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I42" s="1"/>
     </row>
@@ -1064,13 +1080,13 @@
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G43" s="1">
         <v>0</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I43" s="1"/>
     </row>
@@ -1080,13 +1096,13 @@
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G44" s="1">
         <v>0</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I44" s="1"/>
     </row>
@@ -1096,13 +1112,13 @@
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G45" s="1">
         <v>0</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I45" s="1"/>
     </row>
@@ -1112,13 +1128,13 @@
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G46" s="1">
         <v>0</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I46" s="1"/>
     </row>
@@ -1128,13 +1144,13 @@
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G47" s="1">
         <v>0</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I47" s="1"/>
     </row>
@@ -1144,13 +1160,13 @@
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G48" s="1">
         <v>0</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I48" s="1"/>
     </row>
@@ -1160,13 +1176,13 @@
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G49" s="1">
         <v>0</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I49" s="1"/>
     </row>
@@ -1176,13 +1192,13 @@
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G50" s="1">
         <v>0</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I50" s="1"/>
     </row>
@@ -1192,13 +1208,13 @@
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G51" s="1">
         <v>0</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I51" s="1"/>
     </row>
@@ -1208,13 +1224,13 @@
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G52" s="1">
         <v>0</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I52" s="1"/>
     </row>
@@ -1224,16 +1240,16 @@
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G53" s="3">
         <v>60</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="4:9" x14ac:dyDescent="0.25">
@@ -1242,14 +1258,14 @@
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G54" s="1">
         <f>G6+1</f>
         <v>64</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I54" s="1"/>
     </row>
@@ -1259,14 +1275,14 @@
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G55" s="1">
         <f>G7+1</f>
         <v>67</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I55" s="1"/>
     </row>
@@ -1276,14 +1292,14 @@
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G56" s="1">
         <f>G8+1</f>
         <v>71</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I56" s="1"/>
     </row>
@@ -1293,14 +1309,14 @@
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G57" s="1">
         <f>G9+1</f>
         <v>74</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I57" s="1"/>
     </row>
@@ -1310,14 +1326,14 @@
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G58" s="1">
         <f>G18+1</f>
         <v>77</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I58" s="1"/>
     </row>
@@ -1327,14 +1343,14 @@
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G59" s="1">
         <f>G11+1</f>
         <v>81</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I59" s="1"/>
     </row>
@@ -1344,13 +1360,13 @@
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G60" s="1">
         <v>0</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I60" s="1"/>
     </row>
@@ -1360,14 +1376,14 @@
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G61" s="1">
         <f>G53+1</f>
         <v>61</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I61" s="1"/>
     </row>
@@ -1377,13 +1393,13 @@
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G62" s="1">
         <v>0</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I62" s="1"/>
     </row>
@@ -1393,14 +1409,14 @@
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G63" s="1">
         <f>G55+1</f>
         <v>68</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I63" s="1"/>
     </row>
@@ -1410,13 +1426,13 @@
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G64" s="1">
         <v>0</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I64" s="1"/>
     </row>
@@ -1426,14 +1442,14 @@
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G65" s="1">
         <f>G57+1</f>
         <v>75</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I65" s="1"/>
     </row>
@@ -1443,14 +1459,14 @@
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G66" s="1">
         <f>G58+1</f>
         <v>78</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I66" s="1"/>
     </row>
@@ -1460,14 +1476,14 @@
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G67" s="1">
         <f>G59+1</f>
         <v>82</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I67" s="1"/>
     </row>
@@ -1477,31 +1493,31 @@
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G68" s="1">
         <v>0</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I68" s="1"/>
     </row>
     <row r="69" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D69">
+      <c r="D69" s="5">
         <v>64</v>
       </c>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G69" s="1">
-        <v>0</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I69" s="1" t="s">
+      <c r="E69" s="5"/>
+      <c r="F69" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G69" s="5">
+        <v>0</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I69" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1511,13 +1527,13 @@
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G70" s="1">
         <v>0</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I70" s="1"/>
     </row>
@@ -1527,13 +1543,13 @@
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G71" s="1">
         <v>0</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I71" s="1"/>
     </row>
@@ -1543,13 +1559,13 @@
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G72" s="1">
         <v>0</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I72" s="1"/>
     </row>
@@ -1559,13 +1575,13 @@
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G73" s="1">
         <v>0</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I73" s="1"/>
     </row>
@@ -1575,13 +1591,13 @@
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G74" s="1">
         <v>0</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I74" s="1"/>
     </row>
@@ -1591,13 +1607,13 @@
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G75" s="1">
         <v>0</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I75" s="1"/>
     </row>
@@ -1607,13 +1623,13 @@
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G76" s="1">
         <v>0</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I76" s="1"/>
     </row>
@@ -1623,13 +1639,13 @@
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G77" s="1">
         <v>0</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I77" s="1"/>
     </row>
@@ -1639,13 +1655,13 @@
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G78" s="1">
         <v>0</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I78" s="1"/>
     </row>
@@ -1655,13 +1671,13 @@
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G79" s="1">
         <v>0</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I79" s="1"/>
     </row>
@@ -1671,13 +1687,13 @@
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G80" s="1">
         <v>0</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I80" s="1"/>
     </row>
@@ -1687,13 +1703,13 @@
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G81" s="1">
         <v>0</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I81" s="1"/>
     </row>
@@ -1703,13 +1719,13 @@
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G82" s="1">
         <v>0</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I82" s="1"/>
     </row>
@@ -1719,13 +1735,13 @@
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G83" s="1">
         <v>0</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I83" s="1"/>
     </row>
@@ -1735,13 +1751,13 @@
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G84" s="1">
         <v>0</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I84" s="1"/>
     </row>
@@ -1751,13 +1767,13 @@
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G85" s="1">
         <v>0</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I85" s="1"/>
     </row>
@@ -1767,13 +1783,13 @@
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G86" s="1">
         <v>0</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I86" s="1"/>
     </row>
@@ -1783,13 +1799,13 @@
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G87" s="1">
         <v>0</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I87" s="1"/>
     </row>
@@ -1799,13 +1815,13 @@
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G88" s="1">
         <v>0</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I88" s="1"/>
     </row>
@@ -1815,13 +1831,13 @@
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G89" s="1">
         <v>0</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I89" s="1"/>
     </row>
@@ -1831,13 +1847,13 @@
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G90" s="1">
         <v>0</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I90" s="1"/>
     </row>
@@ -1847,13 +1863,13 @@
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G91" s="1">
         <v>0</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I91" s="1"/>
     </row>
@@ -1863,13 +1879,13 @@
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G92" s="1">
         <v>0</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I92" s="1"/>
     </row>
@@ -1879,13 +1895,13 @@
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G93" s="1">
         <v>0</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I93" s="1"/>
     </row>
@@ -1895,13 +1911,13 @@
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G94" s="1">
         <v>0</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I94" s="1"/>
     </row>
@@ -1911,13 +1927,13 @@
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G95" s="1">
         <v>0</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I95" s="1"/>
     </row>
@@ -1927,13 +1943,13 @@
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G96" s="1">
         <v>0</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I96" s="1"/>
     </row>
@@ -1943,13 +1959,13 @@
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G97" s="1">
         <v>0</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I97" s="1"/>
     </row>
@@ -1959,13 +1975,13 @@
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G98" s="1">
         <v>0</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I98" s="1"/>
     </row>
@@ -1975,13 +1991,13 @@
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G99" s="1">
         <v>0</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I99" s="1"/>
     </row>
@@ -1991,13 +2007,13 @@
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G100" s="1">
         <v>0</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I100" s="1"/>
     </row>
@@ -2007,13 +2023,13 @@
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G101" s="1">
         <v>0</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I101" s="1"/>
     </row>
@@ -2023,13 +2039,13 @@
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G102" s="1">
         <v>0</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I102" s="1"/>
     </row>
@@ -2039,13 +2055,13 @@
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G103" s="1">
         <v>0</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I103" s="1"/>
     </row>
@@ -2055,13 +2071,13 @@
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G104" s="1">
         <v>0</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I104" s="1"/>
     </row>
@@ -2071,13 +2087,13 @@
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G105" s="1">
         <v>0</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I105" s="1"/>
     </row>
@@ -2087,13 +2103,13 @@
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G106" s="1">
         <v>0</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I106" s="1"/>
     </row>
@@ -2103,13 +2119,13 @@
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G107" s="1">
         <v>0</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I107" s="1"/>
     </row>
@@ -2119,13 +2135,13 @@
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G108" s="1">
         <v>0</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I108" s="1"/>
     </row>
@@ -2135,13 +2151,13 @@
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G109" s="1">
         <v>0</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I109" s="1"/>
     </row>
@@ -2151,13 +2167,13 @@
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G110" s="1">
         <v>0</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I110" s="1"/>
     </row>
@@ -2167,13 +2183,13 @@
       </c>
       <c r="E111" s="1"/>
       <c r="F111" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G111" s="1">
         <v>0</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I111" s="1"/>
     </row>
@@ -2183,13 +2199,13 @@
       </c>
       <c r="E112" s="1"/>
       <c r="F112" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G112" s="1">
         <v>0</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I112" s="1"/>
     </row>
@@ -2199,13 +2215,13 @@
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G113" s="1">
         <v>0</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I113" s="1"/>
     </row>
@@ -2215,13 +2231,13 @@
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G114" s="1">
         <v>0</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I114" s="1"/>
     </row>
@@ -2231,13 +2247,13 @@
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G115" s="1">
         <v>0</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I115" s="1"/>
     </row>
@@ -2247,13 +2263,13 @@
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G116" s="1">
         <v>0</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I116" s="1"/>
     </row>
@@ -2263,13 +2279,13 @@
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G117" s="1">
         <v>0</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I117" s="1"/>
     </row>
@@ -2279,13 +2295,13 @@
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G118" s="1">
         <v>0</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I118" s="1"/>
     </row>
@@ -2295,13 +2311,13 @@
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G119" s="1">
         <v>0</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I119" s="1"/>
     </row>
@@ -2311,13 +2327,13 @@
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G120" s="1">
         <v>0</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I120" s="1"/>
     </row>
@@ -2327,13 +2343,13 @@
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G121" s="1">
         <v>0</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I121" s="1"/>
     </row>
@@ -2343,13 +2359,13 @@
       </c>
       <c r="E122" s="1"/>
       <c r="F122" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G122" s="1">
         <v>0</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I122" s="1"/>
     </row>
@@ -2359,13 +2375,13 @@
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G123" s="1">
         <v>0</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I123" s="1"/>
     </row>
@@ -2375,13 +2391,13 @@
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G124" s="1">
         <v>0</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I124" s="1"/>
     </row>
@@ -2391,13 +2407,13 @@
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G125" s="1">
         <v>0</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I125" s="1"/>
     </row>
@@ -2407,13 +2423,13 @@
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G126" s="1">
         <v>0</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I126" s="1"/>
     </row>
@@ -2423,13 +2439,13 @@
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G127" s="1">
         <v>0</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I127" s="1"/>
     </row>
@@ -2439,13 +2455,13 @@
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G128" s="1">
         <v>0</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I128" s="1"/>
     </row>
@@ -2455,13 +2471,13 @@
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G129" s="1">
         <v>0</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I129" s="1"/>
     </row>
@@ -2471,13 +2487,13 @@
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G130" s="1">
         <v>0</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I130" s="1"/>
     </row>
@@ -2487,13 +2503,13 @@
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G131" s="1">
         <v>0</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I131" s="1"/>
     </row>
@@ -2503,13 +2519,13 @@
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G132" s="1">
         <v>0</v>
       </c>
       <c r="H132" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I132" s="1"/>
     </row>
@@ -2519,13 +2535,13 @@
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G133" s="1">
         <v>0</v>
       </c>
       <c r="H133" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I133" s="1"/>
     </row>
@@ -2535,13 +2551,13 @@
       </c>
       <c r="E134" s="1"/>
       <c r="F134" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G134" s="1">
         <v>0</v>
       </c>
       <c r="H134" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I134" s="1"/>
     </row>
@@ -2551,13 +2567,13 @@
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G135" s="1">
         <v>0</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I135" s="1"/>
     </row>
@@ -2567,13 +2583,13 @@
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G136" s="1">
         <v>0</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I136" s="1"/>
     </row>
@@ -2583,13 +2599,13 @@
       </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G137" s="1">
         <v>0</v>
       </c>
       <c r="H137" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I137" s="1"/>
     </row>
@@ -2599,13 +2615,13 @@
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G138" s="1">
         <v>0</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I138" s="1"/>
     </row>
@@ -2615,13 +2631,13 @@
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G139" s="1">
         <v>0</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I139" s="1"/>
     </row>
@@ -2631,13 +2647,13 @@
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G140" s="1">
         <v>0</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I140" s="1"/>
     </row>
@@ -2647,13 +2663,13 @@
       </c>
       <c r="E141" s="1"/>
       <c r="F141" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G141" s="1">
         <v>0</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I141" s="1"/>
     </row>
@@ -2663,13 +2679,13 @@
       </c>
       <c r="E142" s="1"/>
       <c r="F142" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G142" s="1">
         <v>0</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I142" s="1"/>
     </row>
@@ -2679,13 +2695,13 @@
       </c>
       <c r="E143" s="1"/>
       <c r="F143" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G143" s="1">
         <v>0</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I143" s="1"/>
     </row>
@@ -2695,13 +2711,13 @@
       </c>
       <c r="E144" s="1"/>
       <c r="F144" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G144" s="1">
         <v>0</v>
       </c>
       <c r="H144" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I144" s="1"/>
     </row>
@@ -2711,13 +2727,13 @@
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G145" s="1">
         <v>0</v>
       </c>
       <c r="H145" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I145" s="1"/>
     </row>
@@ -2727,13 +2743,13 @@
       </c>
       <c r="E146" s="1"/>
       <c r="F146" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G146" s="1">
         <v>0</v>
       </c>
       <c r="H146" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I146" s="1"/>
     </row>
@@ -2743,13 +2759,13 @@
       </c>
       <c r="E147" s="1"/>
       <c r="F147" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G147" s="1">
         <v>0</v>
       </c>
       <c r="H147" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I147" s="1"/>
     </row>
@@ -2759,13 +2775,13 @@
       </c>
       <c r="E148" s="1"/>
       <c r="F148" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G148" s="1">
         <v>0</v>
       </c>
       <c r="H148" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I148" s="1"/>
     </row>
@@ -2775,13 +2791,13 @@
       </c>
       <c r="E149" s="1"/>
       <c r="F149" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G149" s="1">
         <v>0</v>
       </c>
       <c r="H149" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I149" s="1"/>
     </row>
@@ -2791,13 +2807,13 @@
       </c>
       <c r="E150" s="1"/>
       <c r="F150" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G150" s="1">
         <v>0</v>
       </c>
       <c r="H150" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I150" s="1"/>
     </row>
@@ -2807,13 +2823,13 @@
       </c>
       <c r="E151" s="1"/>
       <c r="F151" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G151" s="1">
         <v>0</v>
       </c>
       <c r="H151" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I151" s="1"/>
     </row>
@@ -2823,13 +2839,13 @@
       </c>
       <c r="E152" s="1"/>
       <c r="F152" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G152" s="1">
         <v>0</v>
       </c>
       <c r="H152" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I152" s="1"/>
     </row>
@@ -2839,13 +2855,13 @@
       </c>
       <c r="E153" s="1"/>
       <c r="F153" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G153" s="1">
         <v>0</v>
       </c>
       <c r="H153" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I153" s="1"/>
     </row>
@@ -2855,13 +2871,13 @@
       </c>
       <c r="E154" s="1"/>
       <c r="F154" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G154" s="1">
         <v>0</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I154" s="1"/>
     </row>
@@ -2871,13 +2887,13 @@
       </c>
       <c r="E155" s="1"/>
       <c r="F155" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G155" s="1">
         <v>0</v>
       </c>
       <c r="H155" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I155" s="1"/>
     </row>
@@ -2887,13 +2903,13 @@
       </c>
       <c r="E156" s="1"/>
       <c r="F156" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G156" s="1">
         <v>0</v>
       </c>
       <c r="H156" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I156" s="1"/>
     </row>
@@ -2903,13 +2919,13 @@
       </c>
       <c r="E157" s="1"/>
       <c r="F157" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G157" s="1">
         <v>0</v>
       </c>
       <c r="H157" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I157" s="1"/>
     </row>
@@ -2919,13 +2935,13 @@
       </c>
       <c r="E158" s="1"/>
       <c r="F158" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G158" s="1">
         <v>0</v>
       </c>
       <c r="H158" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I158" s="1"/>
     </row>
@@ -2935,13 +2951,13 @@
       </c>
       <c r="E159" s="1"/>
       <c r="F159" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G159" s="1">
         <v>0</v>
       </c>
       <c r="H159" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I159" s="1"/>
     </row>
@@ -2951,13 +2967,13 @@
       </c>
       <c r="E160" s="1"/>
       <c r="F160" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G160" s="1">
         <v>0</v>
       </c>
       <c r="H160" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I160" s="1"/>
     </row>
@@ -2967,13 +2983,13 @@
       </c>
       <c r="E161" s="1"/>
       <c r="F161" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G161" s="1">
         <v>0</v>
       </c>
       <c r="H161" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I161" s="1"/>
     </row>
@@ -2983,13 +2999,13 @@
       </c>
       <c r="E162" s="1"/>
       <c r="F162" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G162" s="1">
         <v>0</v>
       </c>
       <c r="H162" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I162" s="1"/>
     </row>
@@ -2999,13 +3015,13 @@
       </c>
       <c r="E163" s="1"/>
       <c r="F163" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G163" s="1">
         <v>0</v>
       </c>
       <c r="H163" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I163" s="1"/>
     </row>
@@ -3015,13 +3031,13 @@
       </c>
       <c r="E164" s="1"/>
       <c r="F164" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G164" s="1">
         <v>0</v>
       </c>
       <c r="H164" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I164" s="1"/>
     </row>
@@ -3031,13 +3047,13 @@
       </c>
       <c r="E165" s="1"/>
       <c r="F165" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G165" s="1">
         <v>0</v>
       </c>
       <c r="H165" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I165" s="1"/>
     </row>
@@ -3047,13 +3063,13 @@
       </c>
       <c r="E166" s="1"/>
       <c r="F166" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G166" s="1">
         <v>0</v>
       </c>
       <c r="H166" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I166" s="1"/>
     </row>
@@ -3063,13 +3079,13 @@
       </c>
       <c r="E167" s="1"/>
       <c r="F167" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G167" s="1">
         <v>0</v>
       </c>
       <c r="H167" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I167" s="1"/>
     </row>
@@ -3079,13 +3095,13 @@
       </c>
       <c r="E168" s="1"/>
       <c r="F168" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G168" s="1">
         <v>0</v>
       </c>
       <c r="H168" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I168" s="1"/>
     </row>
@@ -3095,13 +3111,13 @@
       </c>
       <c r="E169" s="1"/>
       <c r="F169" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G169" s="1">
         <v>0</v>
       </c>
       <c r="H169" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I169" s="1"/>
     </row>
@@ -3111,13 +3127,13 @@
       </c>
       <c r="E170" s="1"/>
       <c r="F170" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G170" s="1">
         <v>0</v>
       </c>
       <c r="H170" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I170" s="1"/>
     </row>
@@ -3127,13 +3143,13 @@
       </c>
       <c r="E171" s="1"/>
       <c r="F171" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G171" s="1">
         <v>0</v>
       </c>
       <c r="H171" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I171" s="1"/>
     </row>
@@ -3143,13 +3159,13 @@
       </c>
       <c r="E172" s="1"/>
       <c r="F172" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G172" s="1">
         <v>0</v>
       </c>
       <c r="H172" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I172" s="1"/>
     </row>
@@ -3159,13 +3175,13 @@
       </c>
       <c r="E173" s="1"/>
       <c r="F173" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G173" s="1">
         <v>0</v>
       </c>
       <c r="H173" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I173" s="1"/>
     </row>
@@ -3175,13 +3191,13 @@
       </c>
       <c r="E174" s="1"/>
       <c r="F174" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G174" s="1">
         <v>0</v>
       </c>
       <c r="H174" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I174" s="1"/>
     </row>
@@ -3191,13 +3207,13 @@
       </c>
       <c r="E175" s="1"/>
       <c r="F175" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G175" s="1">
         <v>0</v>
       </c>
       <c r="H175" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I175" s="1"/>
     </row>
@@ -3207,13 +3223,13 @@
       </c>
       <c r="E176" s="1"/>
       <c r="F176" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G176" s="1">
         <v>0</v>
       </c>
       <c r="H176" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I176" s="1"/>
     </row>
@@ -3223,13 +3239,13 @@
       </c>
       <c r="E177" s="1"/>
       <c r="F177" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G177" s="1">
         <v>0</v>
       </c>
       <c r="H177" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I177" s="1"/>
     </row>
@@ -3239,13 +3255,13 @@
       </c>
       <c r="E178" s="1"/>
       <c r="F178" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G178" s="1">
         <v>0</v>
       </c>
       <c r="H178" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I178" s="1"/>
     </row>
@@ -3255,13 +3271,13 @@
       </c>
       <c r="E179" s="1"/>
       <c r="F179" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G179" s="1">
         <v>0</v>
       </c>
       <c r="H179" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I179" s="1"/>
     </row>
@@ -3271,13 +3287,13 @@
       </c>
       <c r="E180" s="1"/>
       <c r="F180" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G180" s="1">
         <v>0</v>
       </c>
       <c r="H180" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I180" s="1"/>
     </row>
@@ -3287,13 +3303,13 @@
       </c>
       <c r="E181" s="1"/>
       <c r="F181" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G181" s="1">
         <v>0</v>
       </c>
       <c r="H181" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I181" s="1"/>
     </row>
@@ -3303,13 +3319,13 @@
       </c>
       <c r="E182" s="1"/>
       <c r="F182" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G182" s="1">
         <v>0</v>
       </c>
       <c r="H182" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I182" s="1"/>
     </row>
@@ -3319,13 +3335,13 @@
       </c>
       <c r="E183" s="1"/>
       <c r="F183" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G183" s="1">
         <v>0</v>
       </c>
       <c r="H183" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I183" s="1"/>
     </row>
@@ -3335,13 +3351,13 @@
       </c>
       <c r="E184" s="1"/>
       <c r="F184" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G184" s="1">
         <v>0</v>
       </c>
       <c r="H184" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I184" s="1"/>
     </row>
@@ -3351,13 +3367,13 @@
       </c>
       <c r="E185" s="1"/>
       <c r="F185" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G185" s="1">
         <v>0</v>
       </c>
       <c r="H185" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I185" s="1"/>
     </row>
@@ -3367,13 +3383,13 @@
       </c>
       <c r="E186" s="1"/>
       <c r="F186" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G186" s="1">
         <v>0</v>
       </c>
       <c r="H186" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I186" s="1"/>
     </row>
@@ -3383,13 +3399,13 @@
       </c>
       <c r="E187" s="1"/>
       <c r="F187" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G187" s="1">
         <v>0</v>
       </c>
       <c r="H187" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I187" s="1"/>
     </row>
@@ -3399,13 +3415,13 @@
       </c>
       <c r="E188" s="1"/>
       <c r="F188" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G188" s="1">
         <v>0</v>
       </c>
       <c r="H188" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I188" s="1"/>
     </row>
@@ -3415,13 +3431,13 @@
       </c>
       <c r="E189" s="1"/>
       <c r="F189" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G189" s="1">
         <v>0</v>
       </c>
       <c r="H189" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I189" s="1"/>
     </row>
@@ -3431,13 +3447,13 @@
       </c>
       <c r="E190" s="1"/>
       <c r="F190" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G190" s="1">
         <v>0</v>
       </c>
       <c r="H190" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I190" s="1"/>
     </row>
@@ -3447,13 +3463,13 @@
       </c>
       <c r="E191" s="1"/>
       <c r="F191" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G191" s="1">
         <v>0</v>
       </c>
       <c r="H191" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I191" s="1"/>
     </row>
@@ -3463,13 +3479,13 @@
       </c>
       <c r="E192" s="1"/>
       <c r="F192" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G192" s="1">
         <v>0</v>
       </c>
       <c r="H192" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I192" s="1"/>
     </row>
@@ -3479,13 +3495,13 @@
       </c>
       <c r="E193" s="1"/>
       <c r="F193" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G193" s="1">
         <v>0</v>
       </c>
       <c r="H193" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I193" s="1"/>
     </row>
@@ -3495,13 +3511,13 @@
       </c>
       <c r="E194" s="1"/>
       <c r="F194" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G194" s="1">
         <v>0</v>
       </c>
       <c r="H194" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I194" s="1"/>
     </row>
@@ -3511,13 +3527,13 @@
       </c>
       <c r="E195" s="1"/>
       <c r="F195" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G195" s="1">
         <v>0</v>
       </c>
       <c r="H195" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I195" s="1"/>
     </row>
@@ -3527,13 +3543,13 @@
       </c>
       <c r="E196" s="1"/>
       <c r="F196" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G196" s="1">
         <v>0</v>
       </c>
       <c r="H196" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I196" s="1"/>
     </row>
@@ -3543,13 +3559,13 @@
       </c>
       <c r="E197" s="1"/>
       <c r="F197" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G197" s="1">
         <v>0</v>
       </c>
       <c r="H197" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I197" s="1"/>
     </row>
@@ -3559,13 +3575,13 @@
       </c>
       <c r="E198" s="1"/>
       <c r="F198" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G198" s="1">
         <v>0</v>
       </c>
       <c r="H198" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I198" s="1"/>
     </row>
@@ -3575,13 +3591,13 @@
       </c>
       <c r="E199" s="1"/>
       <c r="F199" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G199" s="1">
         <v>0</v>
       </c>
       <c r="H199" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I199" s="1"/>
     </row>
@@ -3591,13 +3607,13 @@
       </c>
       <c r="E200" s="1"/>
       <c r="F200" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G200" s="1">
         <v>0</v>
       </c>
       <c r="H200" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I200" s="1"/>
     </row>
@@ -3607,13 +3623,13 @@
       </c>
       <c r="E201" s="1"/>
       <c r="F201" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G201" s="1">
         <v>0</v>
       </c>
       <c r="H201" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I201" s="1"/>
     </row>
@@ -3623,13 +3639,13 @@
       </c>
       <c r="E202" s="1"/>
       <c r="F202" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G202" s="1">
         <v>0</v>
       </c>
       <c r="H202" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I202" s="1"/>
     </row>
@@ -3639,13 +3655,13 @@
       </c>
       <c r="E203" s="1"/>
       <c r="F203" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G203" s="1">
         <v>0</v>
       </c>
       <c r="H203" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I203" s="1"/>
     </row>
@@ -3655,13 +3671,13 @@
       </c>
       <c r="E204" s="1"/>
       <c r="F204" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G204" s="1">
         <v>0</v>
       </c>
       <c r="H204" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I204" s="1"/>
     </row>
@@ -3671,13 +3687,13 @@
       </c>
       <c r="E205" s="1"/>
       <c r="F205" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G205" s="1">
         <v>0</v>
       </c>
       <c r="H205" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I205" s="1"/>
     </row>
@@ -3687,13 +3703,13 @@
       </c>
       <c r="E206" s="1"/>
       <c r="F206" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G206" s="1">
         <v>0</v>
       </c>
       <c r="H206" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I206" s="1"/>
     </row>
@@ -3703,13 +3719,13 @@
       </c>
       <c r="E207" s="1"/>
       <c r="F207" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G207" s="1">
         <v>0</v>
       </c>
       <c r="H207" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I207" s="1"/>
     </row>
@@ -3719,13 +3735,13 @@
       </c>
       <c r="E208" s="1"/>
       <c r="F208" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G208" s="1">
         <v>0</v>
       </c>
       <c r="H208" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I208" s="1"/>
     </row>
@@ -3735,13 +3751,13 @@
       </c>
       <c r="E209" s="1"/>
       <c r="F209" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G209" s="1">
         <v>0</v>
       </c>
       <c r="H209" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I209" s="1"/>
     </row>
@@ -3751,13 +3767,13 @@
       </c>
       <c r="E210" s="1"/>
       <c r="F210" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G210" s="1">
         <v>0</v>
       </c>
       <c r="H210" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I210" s="1"/>
     </row>
@@ -3767,13 +3783,13 @@
       </c>
       <c r="E211" s="1"/>
       <c r="F211" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G211" s="1">
         <v>0</v>
       </c>
       <c r="H211" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I211" s="1"/>
     </row>
@@ -3783,13 +3799,13 @@
       </c>
       <c r="E212" s="1"/>
       <c r="F212" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G212" s="1">
         <v>0</v>
       </c>
       <c r="H212" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I212" s="1"/>
     </row>
@@ -3799,13 +3815,13 @@
       </c>
       <c r="E213" s="1"/>
       <c r="F213" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G213" s="1">
         <v>0</v>
       </c>
       <c r="H213" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I213" s="1"/>
     </row>
@@ -3815,13 +3831,13 @@
       </c>
       <c r="E214" s="1"/>
       <c r="F214" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G214" s="1">
         <v>0</v>
       </c>
       <c r="H214" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I214" s="1"/>
     </row>
@@ -3831,13 +3847,13 @@
       </c>
       <c r="E215" s="1"/>
       <c r="F215" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G215" s="1">
         <v>0</v>
       </c>
       <c r="H215" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I215" s="1"/>
     </row>
@@ -3847,13 +3863,13 @@
       </c>
       <c r="E216" s="1"/>
       <c r="F216" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G216" s="1">
         <v>0</v>
       </c>
       <c r="H216" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I216" s="1"/>
     </row>
@@ -3863,13 +3879,13 @@
       </c>
       <c r="E217" s="1"/>
       <c r="F217" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G217" s="1">
         <v>0</v>
       </c>
       <c r="H217" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I217" s="1"/>
     </row>
@@ -3879,13 +3895,13 @@
       </c>
       <c r="E218" s="1"/>
       <c r="F218" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G218" s="1">
         <v>0</v>
       </c>
       <c r="H218" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I218" s="1"/>
     </row>
@@ -3895,13 +3911,13 @@
       </c>
       <c r="E219" s="1"/>
       <c r="F219" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G219" s="1">
         <v>0</v>
       </c>
       <c r="H219" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I219" s="1"/>
     </row>
@@ -3911,13 +3927,13 @@
       </c>
       <c r="E220" s="1"/>
       <c r="F220" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G220" s="1">
         <v>0</v>
       </c>
       <c r="H220" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I220" s="1"/>
     </row>
@@ -3927,13 +3943,13 @@
       </c>
       <c r="E221" s="1"/>
       <c r="F221" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G221" s="1">
         <v>0</v>
       </c>
       <c r="H221" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I221" s="1"/>
     </row>
@@ -3943,13 +3959,13 @@
       </c>
       <c r="E222" s="1"/>
       <c r="F222" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G222" s="1">
         <v>0</v>
       </c>
       <c r="H222" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I222" s="1"/>
     </row>
@@ -3959,13 +3975,13 @@
       </c>
       <c r="E223" s="1"/>
       <c r="F223" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G223" s="1">
         <v>0</v>
       </c>
       <c r="H223" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I223" s="1"/>
     </row>
@@ -3975,13 +3991,13 @@
       </c>
       <c r="E224" s="1"/>
       <c r="F224" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G224" s="1">
         <v>0</v>
       </c>
       <c r="H224" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I224" s="1"/>
     </row>
@@ -3991,13 +4007,13 @@
       </c>
       <c r="E225" s="1"/>
       <c r="F225" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G225" s="1">
         <v>0</v>
       </c>
       <c r="H225" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I225" s="1"/>
     </row>
@@ -4007,13 +4023,13 @@
       </c>
       <c r="E226" s="1"/>
       <c r="F226" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G226" s="1">
         <v>0</v>
       </c>
       <c r="H226" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I226" s="1"/>
     </row>
@@ -4023,13 +4039,13 @@
       </c>
       <c r="E227" s="1"/>
       <c r="F227" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G227" s="1">
         <v>0</v>
       </c>
       <c r="H227" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I227" s="1"/>
     </row>
@@ -4039,13 +4055,13 @@
       </c>
       <c r="E228" s="1"/>
       <c r="F228" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G228" s="1">
         <v>0</v>
       </c>
       <c r="H228" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I228" s="1"/>
     </row>
@@ -4055,13 +4071,13 @@
       </c>
       <c r="E229" s="1"/>
       <c r="F229" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G229" s="1">
         <v>0</v>
       </c>
       <c r="H229" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I229" s="1"/>
     </row>
@@ -4071,13 +4087,13 @@
       </c>
       <c r="E230" s="1"/>
       <c r="F230" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G230" s="1">
         <v>0</v>
       </c>
       <c r="H230" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I230" s="1"/>
     </row>
@@ -4087,13 +4103,13 @@
       </c>
       <c r="E231" s="1"/>
       <c r="F231" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G231" s="1">
         <v>0</v>
       </c>
       <c r="H231" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I231" s="1"/>
     </row>
@@ -4103,13 +4119,13 @@
       </c>
       <c r="E232" s="1"/>
       <c r="F232" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G232" s="1">
         <v>0</v>
       </c>
       <c r="H232" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I232" s="1"/>
     </row>
@@ -4119,13 +4135,13 @@
       </c>
       <c r="E233" s="1"/>
       <c r="F233" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G233" s="1">
         <v>0</v>
       </c>
       <c r="H233" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I233" s="1"/>
     </row>
@@ -4135,13 +4151,13 @@
       </c>
       <c r="E234" s="1"/>
       <c r="F234" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G234" s="1">
         <v>0</v>
       </c>
       <c r="H234" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I234" s="1"/>
     </row>
@@ -4151,13 +4167,13 @@
       </c>
       <c r="E235" s="1"/>
       <c r="F235" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G235" s="1">
         <v>0</v>
       </c>
       <c r="H235" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I235" s="1"/>
     </row>
@@ -4167,13 +4183,13 @@
       </c>
       <c r="E236" s="1"/>
       <c r="F236" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G236" s="1">
         <v>0</v>
       </c>
       <c r="H236" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I236" s="1"/>
     </row>
@@ -4183,13 +4199,13 @@
       </c>
       <c r="E237" s="1"/>
       <c r="F237" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G237" s="1">
         <v>0</v>
       </c>
       <c r="H237" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I237" s="1"/>
     </row>
@@ -4199,13 +4215,13 @@
       </c>
       <c r="E238" s="1"/>
       <c r="F238" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G238" s="1">
         <v>0</v>
       </c>
       <c r="H238" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I238" s="1"/>
     </row>
@@ -4215,13 +4231,13 @@
       </c>
       <c r="E239" s="1"/>
       <c r="F239" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G239" s="1">
         <v>0</v>
       </c>
       <c r="H239" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I239" s="1"/>
     </row>
@@ -4231,13 +4247,13 @@
       </c>
       <c r="E240" s="1"/>
       <c r="F240" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G240" s="1">
         <v>0</v>
       </c>
       <c r="H240" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I240" s="1"/>
     </row>
@@ -4247,13 +4263,13 @@
       </c>
       <c r="E241" s="1"/>
       <c r="F241" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G241" s="1">
         <v>0</v>
       </c>
       <c r="H241" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I241" s="1"/>
     </row>
@@ -4263,13 +4279,13 @@
       </c>
       <c r="E242" s="1"/>
       <c r="F242" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G242" s="1">
         <v>0</v>
       </c>
       <c r="H242" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I242" s="1"/>
     </row>
@@ -4279,13 +4295,13 @@
       </c>
       <c r="E243" s="1"/>
       <c r="F243" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G243" s="1">
         <v>0</v>
       </c>
       <c r="H243" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I243" s="1"/>
     </row>
@@ -4295,13 +4311,13 @@
       </c>
       <c r="E244" s="1"/>
       <c r="F244" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G244" s="1">
         <v>0</v>
       </c>
       <c r="H244" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I244" s="1"/>
     </row>
@@ -4311,13 +4327,13 @@
       </c>
       <c r="E245" s="1"/>
       <c r="F245" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G245" s="1">
         <v>0</v>
       </c>
       <c r="H245" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I245" s="1"/>
     </row>
@@ -4327,13 +4343,13 @@
       </c>
       <c r="E246" s="1"/>
       <c r="F246" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G246" s="1">
         <v>0</v>
       </c>
       <c r="H246" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I246" s="1"/>
     </row>
@@ -4343,13 +4359,13 @@
       </c>
       <c r="E247" s="1"/>
       <c r="F247" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G247" s="1">
         <v>0</v>
       </c>
       <c r="H247" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I247" s="1"/>
     </row>
@@ -4359,13 +4375,13 @@
       </c>
       <c r="E248" s="1"/>
       <c r="F248" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G248" s="1">
         <v>0</v>
       </c>
       <c r="H248" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I248" s="1"/>
     </row>
@@ -4375,13 +4391,13 @@
       </c>
       <c r="E249" s="1"/>
       <c r="F249" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G249" s="1">
         <v>0</v>
       </c>
       <c r="H249" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I249" s="1"/>
     </row>
@@ -4391,13 +4407,13 @@
       </c>
       <c r="E250" s="1"/>
       <c r="F250" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G250" s="1">
         <v>0</v>
       </c>
       <c r="H250" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I250" s="1"/>
     </row>
@@ -4407,13 +4423,13 @@
       </c>
       <c r="E251" s="1"/>
       <c r="F251" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G251" s="1">
         <v>0</v>
       </c>
       <c r="H251" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I251" s="1"/>
     </row>
@@ -4423,13 +4439,13 @@
       </c>
       <c r="E252" s="1"/>
       <c r="F252" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G252" s="1">
         <v>0</v>
       </c>
       <c r="H252" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I252" s="1"/>
     </row>
@@ -4439,13 +4455,13 @@
       </c>
       <c r="E253" s="1"/>
       <c r="F253" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G253" s="1">
         <v>0</v>
       </c>
       <c r="H253" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I253" s="1"/>
     </row>
@@ -4455,13 +4471,13 @@
       </c>
       <c r="E254" s="1"/>
       <c r="F254" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G254" s="1">
         <v>0</v>
       </c>
       <c r="H254" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I254" s="1"/>
     </row>
@@ -4471,13 +4487,13 @@
       </c>
       <c r="E255" s="1"/>
       <c r="F255" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G255" s="1">
         <v>0</v>
       </c>
       <c r="H255" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I255" s="1"/>
     </row>
@@ -4487,13 +4503,13 @@
       </c>
       <c r="E256" s="1"/>
       <c r="F256" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G256" s="1">
         <v>0</v>
       </c>
       <c r="H256" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I256" s="1"/>
     </row>
@@ -4503,13 +4519,13 @@
       </c>
       <c r="E257" s="1"/>
       <c r="F257" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G257" s="1">
         <v>0</v>
       </c>
       <c r="H257" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I257" s="1"/>
     </row>
@@ -4519,13 +4535,13 @@
       </c>
       <c r="E258" s="1"/>
       <c r="F258" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G258" s="1">
         <v>0</v>
       </c>
       <c r="H258" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I258" s="1"/>
     </row>
@@ -4535,13 +4551,13 @@
       </c>
       <c r="E259" s="1"/>
       <c r="F259" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G259" s="1">
         <v>0</v>
       </c>
       <c r="H259" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I259" s="1"/>
     </row>
@@ -4551,13 +4567,13 @@
       </c>
       <c r="E260" s="1"/>
       <c r="F260" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G260" s="1">
         <v>0</v>
       </c>
       <c r="H260" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I260" s="1"/>
     </row>

</xml_diff>